<commit_message>
Added readings for https and added wireshark dumps
</commit_message>
<xml_diff>
--- a/reports/HTTPS-Local-ClientSideTime-Streaming-Measurements.xlsx
+++ b/reports/HTTPS-Local-ClientSideTime-Streaming-Measurements.xlsx
@@ -418,10 +418,10 @@
                   <c:v>220.60633333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2076.6085000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4084.0210000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,11 +437,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298895920"/>
-        <c:axId val="298904496"/>
+        <c:axId val="201099528"/>
+        <c:axId val="201099912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298895920"/>
+        <c:axId val="201099528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298904496"/>
+        <c:crossAx val="201099912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -491,7 +491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298904496"/>
+        <c:axId val="201099912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298895920"/>
+        <c:crossAx val="201099528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -796,10 +796,10 @@
                   <c:v>149.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>156.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +815,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="299247008"/>
-        <c:axId val="299247400"/>
+        <c:axId val="158183760"/>
+        <c:axId val="158184152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="299247008"/>
+        <c:axId val="158183760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299247400"/>
+        <c:crossAx val="158184152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -869,7 +869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299247400"/>
+        <c:axId val="158184152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,7 +919,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299247008"/>
+        <c:crossAx val="158183760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1018,7 +1018,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1203,11 +1202,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="299354664"/>
-        <c:axId val="299355056"/>
+        <c:axId val="201845280"/>
+        <c:axId val="201845672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="299354664"/>
+        <c:axId val="201845280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1267,7 +1266,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299355056"/>
+        <c:crossAx val="201845672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1275,7 +1274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299355056"/>
+        <c:axId val="201845672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299354664"/>
+        <c:crossAx val="201845280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1350,7 +1349,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1643,10 +1641,10 @@
                   <c:v>86.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1662,11 +1660,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298940200"/>
-        <c:axId val="299021776"/>
+        <c:axId val="200470896"/>
+        <c:axId val="200487664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298940200"/>
+        <c:axId val="200470896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299021776"/>
+        <c:crossAx val="200487664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299021776"/>
+        <c:axId val="200487664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +1764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298940200"/>
+        <c:crossAx val="200470896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1993,10 +1991,10 @@
                   <c:v>22.753333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>206.47533333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2045.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2074,10 +2072,10 @@
                   <c:v>22.787333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>206.179</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2045.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2096,11 +2094,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298655664"/>
-        <c:axId val="299081024"/>
+        <c:axId val="200563624"/>
+        <c:axId val="200564008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298655664"/>
+        <c:axId val="200563624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2142,7 +2140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299081024"/>
+        <c:crossAx val="200564008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2150,7 +2148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299081024"/>
+        <c:axId val="200564008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2198,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298655664"/>
+        <c:crossAx val="200563624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2512,10 +2510,10 @@
                   <c:v>218.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>99.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2534,11 +2532,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="299118272"/>
-        <c:axId val="299128728"/>
+        <c:axId val="200606864"/>
+        <c:axId val="200607248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="299118272"/>
+        <c:axId val="200606864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299128728"/>
+        <c:crossAx val="200607248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2588,7 +2586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299128728"/>
+        <c:axId val="200607248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +2636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299118272"/>
+        <c:crossAx val="200606864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2865,10 +2863,10 @@
                   <c:v>23.507999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>207.59733333333335</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2083.7939999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2946,10 +2944,10 @@
                   <c:v>23.463666666666665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>207.34433333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2075.502</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3027,10 +3025,10 @@
                   <c:v>23.516000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>207.68800000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2075.364</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3049,11 +3047,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="299172560"/>
-        <c:axId val="299168064"/>
+        <c:axId val="201476760"/>
+        <c:axId val="201591896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="299172560"/>
+        <c:axId val="201476760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3095,7 +3093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299168064"/>
+        <c:crossAx val="201591896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3103,7 +3101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299168064"/>
+        <c:axId val="201591896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3153,7 +3151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299172560"/>
+        <c:crossAx val="201476760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3465,10 +3463,10 @@
                   <c:v>173.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>128.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3487,11 +3485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="299243872"/>
-        <c:axId val="299244264"/>
+        <c:axId val="158181016"/>
+        <c:axId val="158181408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="299243872"/>
+        <c:axId val="158181016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3533,7 +3531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299244264"/>
+        <c:crossAx val="158181408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3541,7 +3539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299244264"/>
+        <c:axId val="158181408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,7 +3589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299243872"/>
+        <c:crossAx val="158181016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3801,10 +3799,10 @@
                   <c:v>25.022000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>229.73766666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2167.1170000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3876,10 +3874,10 @@
                   <c:v>25.048999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>226.631</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2152.9389999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3951,10 +3949,10 @@
                   <c:v>25.321666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>226.99600000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2175.0349999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4026,10 +4024,10 @@
                   <c:v>25.304000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>227.85433333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2187.4490000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4045,11 +4043,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="237514504"/>
-        <c:axId val="237514112"/>
+        <c:axId val="158179840"/>
+        <c:axId val="158179448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="237514504"/>
+        <c:axId val="158179840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,7 +4108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237514112"/>
+        <c:crossAx val="158179448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4118,7 +4116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237514112"/>
+        <c:axId val="158179448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4179,7 +4177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237514504"/>
+        <c:crossAx val="158179840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4466,10 +4464,10 @@
                   <c:v>117.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4485,11 +4483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="237512544"/>
-        <c:axId val="299245048"/>
+        <c:axId val="158178664"/>
+        <c:axId val="158182192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="237512544"/>
+        <c:axId val="158178664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4550,7 +4548,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299245048"/>
+        <c:crossAx val="158182192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4558,7 +4556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299245048"/>
+        <c:axId val="158182192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4619,7 +4617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237512544"/>
+        <c:crossAx val="158178664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4829,10 +4827,10 @@
                   <c:v>28.675999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>278.82733333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2527.1019999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4904,10 +4902,10 @@
                   <c:v>27.820333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>272.83466666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2500.0239999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4979,10 +4977,10 @@
                   <c:v>28.563666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>269.76666666666671</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2493.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5054,10 +5052,10 @@
                   <c:v>28.33966666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>268.26100000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2453.7460000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5129,10 +5127,10 @@
                   <c:v>28.78233333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>276.24299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2531.6280000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5148,11 +5146,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="299245832"/>
-        <c:axId val="299246224"/>
+        <c:axId val="158180624"/>
+        <c:axId val="158182976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="299245832"/>
+        <c:axId val="158180624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5194,7 +5192,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299246224"/>
+        <c:crossAx val="158182976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5202,7 +5200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="299246224"/>
+        <c:axId val="158182976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5252,7 +5250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299245832"/>
+        <c:crossAx val="158180624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12031,8 +12029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12197,13 +12195,21 @@
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1">
+        <v>2111.0430000000001</v>
+      </c>
+      <c r="C18" s="1">
+        <v>123</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="1">
+        <v>2042.174</v>
+      </c>
+      <c r="C19" s="1">
+        <v>79</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -12214,21 +12220,25 @@
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="4" t="e">
+      <c r="B21" s="4">
         <f>AVERAGE(B18:B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="4" t="e">
+        <v>2076.6085000000003</v>
+      </c>
+      <c r="C21" s="4">
         <f t="shared" ref="C21" si="3">AVERAGE(C18:C20)</f>
-        <v>#DIV/0!</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1">
+        <v>4084.0210000000002</v>
+      </c>
+      <c r="C22" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -12244,13 +12254,13 @@
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="4" t="e">
+      <c r="B25" s="4">
         <f>AVERAGE(B22:B24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25" s="4" t="e">
+        <v>4084.0210000000002</v>
+      </c>
+      <c r="C25" s="4">
         <f>AVERAGE(C22:C24)</f>
-        <v>#DIV/0!</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12307,26 +12317,26 @@
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1" t="e">
+      <c r="B34" s="1">
         <f>B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="1" t="e">
+        <v>2076.6085000000003</v>
+      </c>
+      <c r="C34" s="1">
         <f t="shared" ref="C34" si="7">C21</f>
-        <v>#DIV/0!</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="1" t="e">
+      <c r="B35" s="1">
         <f>B25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C35" s="1" t="e">
+        <v>4084.0210000000002</v>
+      </c>
+      <c r="C35" s="1">
         <f t="shared" ref="C35" si="8">C25</f>
-        <v>#DIV/0!</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -12340,7 +12350,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12492,46 +12502,70 @@
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="1">
+        <v>208.40299999999999</v>
+      </c>
+      <c r="C14" s="1">
+        <v>207.74799999999999</v>
+      </c>
+      <c r="D14" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="B15" s="1">
+        <v>205.72800000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>205.68600000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="1">
+        <v>205.29499999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>205.10300000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <v>118</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="e">
+      <c r="B17" s="4">
         <f>AVERAGE(B14:B16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="4" t="e">
+        <v>206.47533333333331</v>
+      </c>
+      <c r="C17" s="4">
         <f t="shared" ref="C17:D17" si="1">AVERAGE(C14:C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="4" t="e">
+        <v>206.179</v>
+      </c>
+      <c r="D17" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>99.333333333333329</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="1">
+        <v>2045.24</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2045.26</v>
+      </c>
+      <c r="D18" s="1">
+        <v>121</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -12549,17 +12583,17 @@
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="4" t="e">
+      <c r="B21" s="4">
         <f>AVERAGE(B18:B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="4" t="e">
+        <v>2045.24</v>
+      </c>
+      <c r="C21" s="4">
         <f t="shared" ref="C21:D21" si="2">AVERAGE(C18:C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" s="4" t="e">
+        <v>2045.26</v>
+      </c>
+      <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -12651,34 +12685,34 @@
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="1" t="e">
+      <c r="B33" s="1">
         <f>B17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" s="1" t="e">
+        <v>206.47533333333331</v>
+      </c>
+      <c r="C33" s="1">
         <f t="shared" ref="C33:D33" si="5">C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" s="1" t="e">
+        <v>206.179</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>99.333333333333329</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1" t="e">
+      <c r="B34" s="1">
         <f>B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="1" t="e">
+        <v>2045.24</v>
+      </c>
+      <c r="C34" s="1">
         <f t="shared" ref="C34:D34" si="6">C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="1" t="e">
+        <v>2045.26</v>
+      </c>
+      <c r="D34" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -12709,7 +12743,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12890,54 +12924,86 @@
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="1">
+        <v>208.62799999999999</v>
+      </c>
+      <c r="C14" s="1">
+        <v>208.56399999999999</v>
+      </c>
+      <c r="D14" s="1">
+        <v>209.11699999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <v>130</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="1">
+        <v>207.09100000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>206.946</v>
+      </c>
+      <c r="D15" s="1">
+        <v>206.59899999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="1">
+        <v>207.07300000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>206.523</v>
+      </c>
+      <c r="D16" s="1">
+        <v>207.34800000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>130</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="e">
+      <c r="B17" s="4">
         <f>AVERAGE(B14:B16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="4" t="e">
+        <v>207.59733333333335</v>
+      </c>
+      <c r="C17" s="4">
         <f t="shared" ref="C17:E17" si="2">AVERAGE(C14:C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="4" t="e">
+        <v>207.34433333333334</v>
+      </c>
+      <c r="D17" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="4" t="e">
+        <v>207.68800000000002</v>
+      </c>
+      <c r="E17" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>128.66666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="1">
+        <v>2083.7939999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2075.502</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2075.364</v>
+      </c>
+      <c r="E18" s="1">
+        <v>161</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -12957,21 +13023,21 @@
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="4" t="e">
+      <c r="B21" s="4">
         <f>AVERAGE(B18:B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="4" t="e">
+        <v>2083.7939999999999</v>
+      </c>
+      <c r="C21" s="4">
         <f t="shared" ref="C21:E21" si="3">AVERAGE(C18:C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" s="4" t="e">
+        <v>2075.502</v>
+      </c>
+      <c r="D21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="4" t="e">
+        <v>2075.364</v>
+      </c>
+      <c r="E21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -13081,42 +13147,42 @@
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="1" t="e">
+      <c r="B33" s="1">
         <f>B17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" s="1" t="e">
+        <v>207.59733333333335</v>
+      </c>
+      <c r="C33" s="1">
         <f t="shared" ref="C33:E33" si="6">C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" s="1" t="e">
+        <v>207.34433333333334</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="1" t="e">
+        <v>207.68800000000002</v>
+      </c>
+      <c r="E33" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>128.66666666666666</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1" t="e">
+      <c r="B34" s="1">
         <f>B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="1" t="e">
+        <v>2083.7939999999999</v>
+      </c>
+      <c r="C34" s="1">
         <f t="shared" ref="C34:E34" si="7">C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="1" t="e">
+        <v>2075.502</v>
+      </c>
+      <c r="D34" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="1" t="e">
+        <v>2075.364</v>
+      </c>
+      <c r="E34" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -13151,7 +13217,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13361,62 +13427,102 @@
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="B14" s="1">
+        <v>250.47300000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>249.76400000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>246.51</v>
+      </c>
+      <c r="E14" s="1">
+        <v>249.78200000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>140</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="B15" s="1">
+        <v>220.71899999999999</v>
+      </c>
+      <c r="C15" s="1">
+        <v>216.35900000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>218.10499999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>217.96700000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>137</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="1">
+        <v>218.02099999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>213.77</v>
+      </c>
+      <c r="D16" s="1">
+        <v>216.37299999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>215.81399999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>146</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="7" t="e">
+      <c r="B17" s="7">
         <f>AVERAGE(B14:B16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="7" t="e">
+        <v>229.73766666666666</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" ref="C17:F17" si="2">AVERAGE(C14:C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="7" t="e">
+        <v>226.631</v>
+      </c>
+      <c r="D17" s="7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="7" t="e">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="E17" s="7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="7" t="e">
+        <v>227.85433333333333</v>
+      </c>
+      <c r="F17" s="7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="B18" s="1">
+        <v>2167.1170000000002</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2152.9389999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2175.0349999999999</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2187.4490000000001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>159</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -13438,25 +13544,25 @@
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="7" t="e">
+      <c r="B21" s="7">
         <f>AVERAGE(B18:B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="7" t="e">
+        <v>2167.1170000000002</v>
+      </c>
+      <c r="C21" s="7">
         <f t="shared" ref="C21:E21" si="3">AVERAGE(C18:C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" s="7" t="e">
+        <v>2152.9389999999999</v>
+      </c>
+      <c r="D21" s="7">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="7" t="e">
+        <v>2175.0349999999999</v>
+      </c>
+      <c r="E21" s="7">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="7" t="e">
+        <v>2187.4490000000001</v>
+      </c>
+      <c r="F21" s="7">
         <f>AVERAGE(F18:F20)</f>
-        <v>#DIV/0!</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -13584,50 +13690,50 @@
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="1" t="e">
+      <c r="B31" s="1">
         <f>B17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C31" s="1" t="e">
+        <v>229.73766666666666</v>
+      </c>
+      <c r="C31" s="1">
         <f t="shared" ref="C31:F31" si="7">C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D31" s="1" t="e">
+        <v>226.631</v>
+      </c>
+      <c r="D31" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="1" t="e">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="E31" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F31" s="1" t="e">
+        <v>227.85433333333333</v>
+      </c>
+      <c r="F31" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="1" t="e">
+      <c r="B32" s="1">
         <f>B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32" s="1" t="e">
+        <v>2167.1170000000002</v>
+      </c>
+      <c r="C32" s="1">
         <f t="shared" ref="C32:F32" si="8">C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D32" s="1" t="e">
+        <v>2152.9389999999999</v>
+      </c>
+      <c r="D32" s="1">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="1" t="e">
+        <v>2175.0349999999999</v>
+      </c>
+      <c r="E32" s="1">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F32" s="1" t="e">
+        <v>2187.4490000000001</v>
+      </c>
+      <c r="F32" s="1">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -13641,7 +13747,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13881,70 +13987,118 @@
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
+      <c r="B14" s="1">
+        <v>287.58</v>
+      </c>
+      <c r="C14" s="1">
+        <v>276.07100000000003</v>
+      </c>
+      <c r="D14" s="1">
+        <v>262.00700000000001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>270.65100000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>279.56700000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>158</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="B15" s="1">
+        <v>270.89499999999998</v>
+      </c>
+      <c r="C15" s="1">
+        <v>270.089</v>
+      </c>
+      <c r="D15" s="1">
+        <v>269.96199999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>264.029</v>
+      </c>
+      <c r="F15" s="1">
+        <v>270.86399999999998</v>
+      </c>
+      <c r="G15" s="2">
+        <v>160</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
+      <c r="B16" s="1">
+        <v>278.00700000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>272.34399999999999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>277.33100000000002</v>
+      </c>
+      <c r="E16" s="1">
+        <v>270.10300000000001</v>
+      </c>
+      <c r="F16" s="1">
+        <v>278.298</v>
+      </c>
+      <c r="G16" s="2">
+        <v>152</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="e">
+      <c r="B17" s="4">
         <f>AVERAGE(B14,B15,B16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="4" t="e">
+        <v>278.82733333333334</v>
+      </c>
+      <c r="C17" s="4">
         <f t="shared" ref="C17:G17" si="2">AVERAGE(C14,C15,C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="4" t="e">
+        <v>272.83466666666669</v>
+      </c>
+      <c r="D17" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="4" t="e">
+        <v>269.76666666666671</v>
+      </c>
+      <c r="E17" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="4" t="e">
+        <v>268.26100000000002</v>
+      </c>
+      <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="4" t="e">
+        <v>276.24299999999999</v>
+      </c>
+      <c r="G17" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>156.66666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="B18" s="1">
+        <v>2527.1019999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2500.0239999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2493.44</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2453.7460000000001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2531.6280000000002</v>
+      </c>
+      <c r="G18" s="1">
+        <v>224</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -13968,29 +14122,29 @@
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="4" t="e">
+      <c r="B21" s="4">
         <f>AVERAGE(B18,B19,B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="4" t="e">
+        <v>2527.1019999999999</v>
+      </c>
+      <c r="C21" s="4">
         <f t="shared" ref="C21:G21" si="3">AVERAGE(C18,C19,C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" s="4" t="e">
+        <v>2500.0239999999999</v>
+      </c>
+      <c r="D21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="4" t="e">
+        <v>2493.44</v>
+      </c>
+      <c r="E21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="4" t="e">
+        <v>2453.7460000000001</v>
+      </c>
+      <c r="F21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="4" t="e">
+        <v>2531.6280000000002</v>
+      </c>
+      <c r="G21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -14078,58 +14232,58 @@
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="1" t="e">
+      <c r="B27" s="1">
         <f>B17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C27" s="1" t="e">
+        <v>278.82733333333334</v>
+      </c>
+      <c r="C27" s="1">
         <f t="shared" ref="C27:G27" si="6">C17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D27" s="1" t="e">
+        <v>272.83466666666669</v>
+      </c>
+      <c r="D27" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="1" t="e">
+        <v>269.76666666666671</v>
+      </c>
+      <c r="E27" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="1" t="e">
+        <v>268.26100000000002</v>
+      </c>
+      <c r="F27" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="1" t="e">
+        <v>276.24299999999999</v>
+      </c>
+      <c r="G27" s="1">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>156.66666666666666</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="1" t="e">
+      <c r="B28" s="1">
         <f>B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" s="1" t="e">
+        <v>2527.1019999999999</v>
+      </c>
+      <c r="C28" s="1">
         <f t="shared" ref="C28:G28" si="7">C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="1" t="e">
+        <v>2500.0239999999999</v>
+      </c>
+      <c r="D28" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="1" t="e">
+        <v>2493.44</v>
+      </c>
+      <c r="E28" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="1" t="e">
+        <v>2453.7460000000001</v>
+      </c>
+      <c r="F28" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="1" t="e">
+        <v>2531.6280000000002</v>
+      </c>
+      <c r="G28" s="1">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>